<commit_message>
add hibernate and jstl. update index.jsp
</commit_message>
<xml_diff>
--- a/doc/database_structure.xlsx
+++ b/doc/database_structure.xlsx
@@ -348,15 +348,16 @@
     <t>PK（自增）</t>
   </si>
   <si>
-    <t>PICTURE_DATA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>图片数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mediumblob</t>
+    <t>varchar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PICTURE_PATH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -725,7 +726,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1033,13 +1034,13 @@
         <v>59</v>
       </c>
       <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="s">
         <v>84</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>86</v>
-      </c>
-      <c r="D27" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:5">

</xml_diff>